<commit_message>
atualização parametros e readme
</commit_message>
<xml_diff>
--- a/Produto - i7.xlsx
+++ b/Produto - i7.xlsx
@@ -1036,68 +1036,68 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Processador Intel Core i7 11700 2.50GHz</t>
+          <t>Processador Intel i7-11700K Rocket Lake 3.60GHz</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>R$ 2.414,61</t>
+          <t>R$ 2.795,31</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/496250/processador-intel-core-i7-11700-2-50ghz</t>
+          <t>https://www.kabum.com.br/produto/497469/processador-intel-i7-11700k-rocket-lake-3-60ghz</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Processador Intel Core i7 10700K 3.80GHz</t>
+          <t>Processador Intel Core i7 11700 2.50GHz</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>R$ 2.335,41</t>
+          <t>R$ 2.414,61</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/496626/processador-intel-core-i7-10700k-3-80ghz</t>
+          <t>https://www.kabum.com.br/produto/496250/processador-intel-core-i7-11700-2-50ghz</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Processador Intel i7-11700K Rocket Lake 3.60GHz</t>
+          <t>Processador Intel Core i7 10700KF 3.80GHz</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>R$ 2.795,31</t>
+          <t>R$ 2.213,91</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/497469/processador-intel-i7-11700k-rocket-lake-3-60ghz</t>
+          <t>https://www.kabum.com.br/produto/497468/processador-intel-core-i7-10700kf-3-80ghz</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Processador Intel Core i7 10700KF 3.80GHz</t>
+          <t>Processador Intel Core i7 10700K 3.80GHz</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>R$ 2.213,91</t>
+          <t>R$ 2.335,41</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/497468/processador-intel-core-i7-10700kf-3-80ghz</t>
+          <t>https://www.kabum.com.br/produto/496626/processador-intel-core-i7-10700k-3-80ghz</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
arrumando utf-8 na conversão
</commit_message>
<xml_diff>
--- a/Produto - i7.xlsx
+++ b/Produto - i7.xlsx
@@ -1053,51 +1053,51 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Processador Intel Core i7 11700 2.50GHz</t>
+          <t>Processador Intel Core i7 10700K 3.80GHz</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>R$ 2.414,61</t>
+          <t>R$ 2.335,41</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/496250/processador-intel-core-i7-11700-2-50ghz</t>
+          <t>https://www.kabum.com.br/produto/496626/processador-intel-core-i7-10700k-3-80ghz</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Processador Intel Core i7 10700KF 3.80GHz</t>
+          <t>Processador Intel Core i7 11700 2.50GHz</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>R$ 2.213,91</t>
+          <t>R$ 2.414,61</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/497468/processador-intel-core-i7-10700kf-3-80ghz</t>
+          <t>https://www.kabum.com.br/produto/496250/processador-intel-core-i7-11700-2-50ghz</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Processador Intel Core i7 10700K 3.80GHz</t>
+          <t>Processador Intel Core i7 10700KF 3.80GHz</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>R$ 2.335,41</t>
+          <t>R$ 2.213,91</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/496626/processador-intel-core-i7-10700k-3-80ghz</t>
+          <t>https://www.kabum.com.br/produto/497468/processador-intel-core-i7-10700kf-3-80ghz</t>
         </is>
       </c>
     </row>

</xml_diff>